<commit_message>
Selenium Season 3 Nov 2nd
</commit_message>
<xml_diff>
--- a/target/test-classes/testdata/excels/regression/Adactin Master Test Data.xlsx
+++ b/target/test-classes/testdata/excels/regression/Adactin Master Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FLM31stJulWS\HybridFrameWork\src\test\resources\testdata\excels\regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1921AAE8-04DF-426F-909F-A30A236BA4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0A4DDD-0639-43B5-BA03-6D32FDEA1736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ECA7341F-7CE3-4EA7-B2BF-C9C26B540FCF}"/>
   </bookViews>
@@ -557,14 +557,14 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5546875" style="1" bestFit="1" customWidth="1"/>

</xml_diff>